<commit_message>
signup and quiz status
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaharshavardhan\Desktop\Resume_Hunter_Api\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B6A8D-5445-4C0B-BEEC-78D28D9A54F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD3EF9A-DF4E-4E78-97DD-4AC35020F66F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -51,13 +51,61 @@
   </si>
   <si>
     <t>"12345678"</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>harsha1222222</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>Subject Expert</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>css</t>
+  </si>
+  <si>
+    <t>vardhan123444</t>
+  </si>
+  <si>
+    <t>vardhan12356666</t>
+  </si>
+  <si>
+    <t>vardhan124444@yopmail.com</t>
+  </si>
+  <si>
+    <t>harsha12344690</t>
+  </si>
+  <si>
+    <t>harsha12389@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +117,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,14 +147,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,14 +519,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AE7678-D804-4C1B-BF5E-12B05B4335DF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{75E8A2AB-C72E-41E4-9BA5-882A3C780A2B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{438EF165-C9E2-426D-994E-07F644B4123D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -488,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E59BB90-572A-452A-BF21-4874D9E7B650}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>

<commit_message>
Api Testing Request Added
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B6A8D-5445-4C0B-BEEC-78D28D9A54F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED6E066-8992-430D-94D6-85A967217068}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -51,13 +51,37 @@
   </si>
   <si>
     <t>"12345678"</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>"30"</t>
+  </si>
+  <si>
+    <t>"1:00"</t>
+  </si>
+  <si>
+    <t>"2022-04-30"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +93,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,14 +130,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,14 +491,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20D81F2-9641-403F-822D-2A1DB6B65379}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4F4D2F4B-DED6-41C4-8A12-B7F5C4521D50}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -488,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E59BB90-572A-452A-BF21-4874D9E7B650}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>

<commit_message>
Api Testing Base Class and Excel file Updated
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED6E066-8992-430D-94D6-85A967217068}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E19E6FA-9DCE-4524-BD96-1F2BA8B47E6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -75,6 +75,54 @@
   </si>
   <si>
     <t>"2022-04-30"</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>harsha1222222</t>
+  </si>
+  <si>
+    <t>harsha12344690</t>
+  </si>
+  <si>
+    <t>harsha12389@yopmail.com</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>vardhan123444</t>
+  </si>
+  <si>
+    <t>vardhan12356666</t>
+  </si>
+  <si>
+    <t>vardhan124444@yopmail.com</t>
+  </si>
+  <si>
+    <t>Subject Expert</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>css</t>
   </si>
 </sst>
 </file>
@@ -493,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20D81F2-9641-403F-822D-2A1DB6B65379}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -544,12 +592,81 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AE7678-D804-4C1B-BF5E-12B05B4335DF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="28.08984375" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>12345678</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>12345678</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Commiting requests without assertion
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksaravanakumar\Documents\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B6A8D-5445-4C0B-BEEC-78D28D9A54F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15765FD2-147A-4C19-AFA4-80658306EAEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="5760" yWindow="24" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -51,6 +51,27 @@
   </si>
   <si>
     <t>"12345678"</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>"3"</t>
+  </si>
+  <si>
+    <t>"78"</t>
+  </si>
+  <si>
+    <t>"2022-04-30"</t>
+  </si>
+  <si>
+    <t>"2022-04-28"</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>integrate analyts29</t>
   </si>
 </sst>
 </file>
@@ -94,9 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,13 +439,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -451,7 +473,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -464,7 +486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -473,12 +495,53 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD5C3E7-F08F-4DB4-BF0A-FCBAD7E3FF98}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -488,9 +551,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E59BB90-572A-452A-BF21-4874D9E7B650}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -503,7 +571,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Api Testing Test Cases Updated
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\IdeaProjects\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\Desktop\Api testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E19E6FA-9DCE-4524-BD96-1F2BA8B47E6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5A5719-77CF-4D6C-83C1-306C5E5C6B17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="270" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Username</t>
   </si>
@@ -123,6 +123,33 @@
   </si>
   <si>
     <t>css</t>
+  </si>
+  <si>
+    <t>1st recr</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>"2022-03-31"</t>
+  </si>
+  <si>
+    <t>Arpit Dadhich</t>
+  </si>
+  <si>
+    <t>arpdadhich@deloitte.com</t>
+  </si>
+  <si>
+    <t>"9765432177"</t>
+  </si>
+  <si>
+    <t>Not Eligible</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Not Selected</t>
   </si>
 </sst>
 </file>
@@ -539,21 +566,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20D81F2-9641-403F-822D-2A1DB6B65379}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,8 +594,10 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -579,6 +609,40 @@
       </c>
       <c r="D2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AE7678-D804-4C1B-BF5E-12B05B4335DF}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test cases for RecruitmentAssignToSubjectExpert
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikck\Desktop\Api testing\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karamjeesingh\Documents\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5A5719-77CF-4D6C-83C1-306C5E5C6B17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DCBC24-0314-48A3-937F-8C816074781E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>Not Selected</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>Shankar1</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -209,12 +227,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -568,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20D81F2-9641-403F-822D-2A1DB6B65379}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -764,12 +791,96 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340587CD-8DEA-453F-8329-1E0605B08426}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>146</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="6">
+        <v>44669</v>
+      </c>
+      <c r="E2" s="6">
+        <v>44674</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated signup and quiz status
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karamjeesingh\Documents\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaharshavardhan\Desktop\Resume_Hunter_Api\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DCBC24-0314-48A3-937F-8C816074781E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C390114-C6C8-4891-BCF7-11E97B12D6B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Username</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>https://somelinkhere</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>2022-04-04</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -227,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -242,6 +254,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -683,15 +699,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AE7678-D804-4C1B-BF5E-12B05B4335DF}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
     <col min="2" max="2" width="17.7265625" customWidth="1"/>
     <col min="3" max="3" width="28.08984375" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
@@ -727,8 +743,8 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>12345678</v>
+      <c r="D2" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -744,8 +760,8 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3">
-        <v>12345678</v>
+      <c r="D3" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -757,9 +773,23 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{BED77B5D-6834-485B-9B06-6E57262EE9CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -793,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340587CD-8DEA-453F-8329-1E0605B08426}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bugs in completed recruitment and recruitment assign to subject expert
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javvkumar\AppData\Local\Temp\MicrosoftEdgeDownloads\6d28bbbc-93fe-407c-9bad-e1194652ca0e\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karamjeesingh\Documents\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4952E5E5-775A-498E-B13E-FE46F51D686E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CB2E99-6980-4E51-81DB-03EC9FEEE78C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Username</t>
   </si>
@@ -171,6 +171,30 @@
   </si>
   <si>
     <t>Quiz Link</t>
+  </si>
+  <si>
+    <t>2022-04-18</t>
+  </si>
+  <si>
+    <t>2022-04-23</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>recruitment_21</t>
+  </si>
+  <si>
+    <t>demo category</t>
+  </si>
+  <si>
+    <t>2022-04-07</t>
+  </si>
+  <si>
+    <t>2022-04-06</t>
   </si>
 </sst>
 </file>
@@ -230,19 +254,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -783,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E59BB90-572A-452A-BF21-4874D9E7B650}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -812,92 +837,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340587CD-8DEA-453F-8329-1E0605B08426}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="16.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>146</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="6">
-        <v>44669</v>
-      </c>
-      <c r="E2" s="6">
-        <v>44674</v>
+      <c r="D2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Merged all the tests and added extent report.
</commit_message>
<xml_diff>
--- a/src/main/resources/apiData.xlsx
+++ b/src/main/resources/apiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javvkumar\AppData\Local\Temp\MicrosoftEdgeDownloads\6d28bbbc-93fe-407c-9bad-e1194652ca0e\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\Automatic-Resume-Filter-Api-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4952E5E5-775A-498E-B13E-FE46F51D686E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295D9E81-514F-4FDD-AED9-BD0EA25A0F83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{DB4806E9-CB77-43F4-9A98-C186B0BFA70C}"/>
   </bookViews>
   <sheets>
     <sheet name="yash" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Username</t>
   </si>
@@ -98,24 +98,12 @@
     <t>harsha1222222</t>
   </si>
   <si>
-    <t>harsha12344690</t>
-  </si>
-  <si>
-    <t>harsha12389@yopmail.com</t>
-  </si>
-  <si>
     <t>HR</t>
   </si>
   <si>
     <t>vardhan123444</t>
   </si>
   <si>
-    <t>vardhan12356666</t>
-  </si>
-  <si>
-    <t>vardhan124444@yopmail.com</t>
-  </si>
-  <si>
     <t>Subject Expert</t>
   </si>
   <si>
@@ -171,6 +159,75 @@
   </si>
   <si>
     <t>Quiz Link</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>recruitment_21</t>
+  </si>
+  <si>
+    <t>demo category</t>
+  </si>
+  <si>
+    <t>2022-04-07</t>
+  </si>
+  <si>
+    <t>2022-04-06</t>
+  </si>
+  <si>
+    <t>2022-04-18</t>
+  </si>
+  <si>
+    <t>2022-04-23</t>
+  </si>
+  <si>
+    <t>https://somelinkhere</t>
+  </si>
+  <si>
+    <t>2022-04-04</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Sdet</t>
+  </si>
+  <si>
+    <t>css,sql,java</t>
+  </si>
+  <si>
+    <t>2022-04-28</t>
+  </si>
+  <si>
+    <t>2022-04-30</t>
+  </si>
+  <si>
+    <t>"3"</t>
+  </si>
+  <si>
+    <t>"78"</t>
+  </si>
+  <si>
+    <t>harsha12344691</t>
+  </si>
+  <si>
+    <t>vardhan12356667</t>
+  </si>
+  <si>
+    <t>harsha12390@yopmail.com</t>
+  </si>
+  <si>
+    <t>vardhan1244456@yopmail.com</t>
+  </si>
+  <si>
+    <t>integration lead12</t>
   </si>
 </sst>
 </file>
@@ -230,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -239,12 +296,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -643,36 +704,36 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -686,15 +747,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AE7678-D804-4C1B-BF5E-12B05B4335DF}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
     <col min="2" max="2" width="17.7265625" customWidth="1"/>
     <col min="3" max="3" width="28.08984375" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
@@ -725,55 +786,112 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>12345678</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3">
-        <v>12345678</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{6AB2A827-8E14-488E-9A23-002CD38DCDEB}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{84B1CD74-84D2-4D01-8059-AE322E583388}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{0B87F05C-C60D-4037-875B-CB20CBCA75B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD5C3E7-F08F-4DB4-BF0A-FCBAD7E3FF98}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -783,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E59BB90-572A-452A-BF21-4874D9E7B650}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -794,7 +912,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -813,56 +931,67 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>146</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="6">
-        <v>44669</v>
-      </c>
-      <c r="E2" s="6">
-        <v>44674</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>

</xml_diff>